<commit_message>
asked questions, replies on to README.md
</commit_message>
<xml_diff>
--- a/Project Backlog for Movies Manager Application.xlsx
+++ b/Project Backlog for Movies Manager Application.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Project: Movie Manager Application by </t>
   </si>
@@ -128,21 +128,21 @@
   <si>
     <t xml:space="preserve">Total Time:</t>
   </si>
-  <si>
-    <t xml:space="preserve">3:36</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="mm:ss"/>
+    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="168" formatCode="0"/>
+    <numFmt numFmtId="169" formatCode="hh:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="170" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -197,6 +197,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF355269"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF355269"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -205,12 +220,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7DC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -263,7 +284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,15 +294,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -289,10 +314,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,36 +329,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,7 +410,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB4C7DC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -401,7 +450,7 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF355269"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -413,15 +462,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4066200</xdr:colOff>
+      <xdr:colOff>4066560</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4701960</xdr:colOff>
+      <xdr:colOff>4701240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>65520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -434,8 +483,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4218480" y="38160"/>
-          <a:ext cx="635760" cy="439200"/>
+          <a:off x="4218120" y="38160"/>
+          <a:ext cx="634680" cy="438120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -455,3159 +504,3290 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="4" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="5" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="7"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="n">
+        <v>0.000694444444444444</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="11" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16" t="n">
+        <v>0.000347222222222222</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11" t="n">
-        <v>0.75</v>
-      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="n">
+        <v>0.000520833333333333</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16" t="n">
+        <v>0.000694444444444444</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="11" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16" t="n">
+        <v>0.000694444444444444</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="H18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="11" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="16" t="n">
+        <v>0.000694444444444444</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="H21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="11" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16" t="n">
+        <v>0.000347222222222222</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="11" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="C24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16" t="n">
+        <v>0.000347222222222222</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16" t="n">
+        <v>0.000694444444444444</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="11" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="C26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="16" t="n">
+        <v>0.000347222222222222</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="H27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="11" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="11" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="11" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="16" t="n">
+        <v>0.000173611111111111</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" s="17" t="n">
+      <c r="D34" s="21" t="n">
+        <f aca="false">SUM(D6:D33)</f>
+        <v>0.00642361111111111</v>
+      </c>
+      <c r="E34" s="22" t="n">
         <f aca="false">SUM(E5:E32)</f>
         <v>0</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="7"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="7"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="7"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="7"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="7"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="7"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="7"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="7"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="7"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="7"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="7"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="7"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="7"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="7"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="7"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="7"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="7"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="7"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="7"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="7"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="7"/>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="7"/>
+      <c r="D57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="7"/>
+      <c r="D58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="7"/>
+      <c r="D59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="7"/>
+      <c r="D60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="7"/>
+      <c r="D61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="7"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="7"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="7"/>
+      <c r="D64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="7"/>
+      <c r="D65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="7"/>
+      <c r="D66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="7"/>
+      <c r="D67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="7"/>
+      <c r="D68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="7"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="7"/>
+      <c r="D70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D71" s="7"/>
+      <c r="D71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="7"/>
+      <c r="D72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="7"/>
+      <c r="D73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="7"/>
+      <c r="D74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D75" s="7"/>
+      <c r="D75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="7"/>
+      <c r="D76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D77" s="7"/>
+      <c r="D77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="7"/>
+      <c r="D78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="7"/>
+      <c r="D79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="7"/>
+      <c r="D80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="7"/>
+      <c r="D81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="7"/>
+      <c r="D82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="7"/>
+      <c r="D83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D84" s="7"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="7"/>
+      <c r="D85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="7"/>
+      <c r="D86" s="8"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="7"/>
+      <c r="D87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="7"/>
+      <c r="D88" s="8"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="7"/>
+      <c r="D89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D90" s="7"/>
+      <c r="D90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="7"/>
+      <c r="D91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="7"/>
+      <c r="D92" s="8"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D93" s="7"/>
+      <c r="D93" s="8"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="7"/>
+      <c r="D94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D95" s="7"/>
+      <c r="D95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D96" s="7"/>
+      <c r="D96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D97" s="7"/>
+      <c r="D97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="7"/>
+      <c r="D98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="7"/>
+      <c r="D99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="7"/>
+      <c r="D100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D101" s="7"/>
+      <c r="D101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="7"/>
+      <c r="D102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="7"/>
+      <c r="D103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="7"/>
+      <c r="D104" s="8"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="7"/>
+      <c r="D105" s="8"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="7"/>
+      <c r="D106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="7"/>
+      <c r="D107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="7"/>
+      <c r="D108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="7"/>
+      <c r="D109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="7"/>
+      <c r="D110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="7"/>
+      <c r="D111" s="8"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="7"/>
+      <c r="D112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="7"/>
+      <c r="D113" s="8"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="7"/>
+      <c r="D114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="7"/>
+      <c r="D115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="7"/>
+      <c r="D116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D117" s="7"/>
+      <c r="D117" s="8"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D118" s="7"/>
+      <c r="D118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D119" s="7"/>
+      <c r="D119" s="8"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D120" s="7"/>
+      <c r="D120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D121" s="7"/>
+      <c r="D121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D122" s="7"/>
+      <c r="D122" s="8"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D123" s="7"/>
+      <c r="D123" s="8"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D124" s="7"/>
+      <c r="D124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D125" s="7"/>
+      <c r="D125" s="8"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D126" s="7"/>
+      <c r="D126" s="8"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D127" s="7"/>
+      <c r="D127" s="8"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D128" s="7"/>
+      <c r="D128" s="8"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D129" s="7"/>
+      <c r="D129" s="8"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D130" s="7"/>
+      <c r="D130" s="8"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D131" s="7"/>
+      <c r="D131" s="8"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D132" s="7"/>
+      <c r="D132" s="8"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D133" s="7"/>
+      <c r="D133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D134" s="7"/>
+      <c r="D134" s="8"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D135" s="7"/>
+      <c r="D135" s="8"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D136" s="7"/>
+      <c r="D136" s="8"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D137" s="7"/>
+      <c r="D137" s="8"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D138" s="7"/>
+      <c r="D138" s="8"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="7"/>
+      <c r="D139" s="8"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="7"/>
+      <c r="D140" s="8"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D141" s="7"/>
+      <c r="D141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D142" s="7"/>
+      <c r="D142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="7"/>
+      <c r="D143" s="8"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D144" s="7"/>
+      <c r="D144" s="8"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D145" s="7"/>
+      <c r="D145" s="8"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D146" s="7"/>
+      <c r="D146" s="8"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D147" s="7"/>
+      <c r="D147" s="8"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D148" s="7"/>
+      <c r="D148" s="8"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D149" s="7"/>
+      <c r="D149" s="8"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D150" s="7"/>
+      <c r="D150" s="8"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D151" s="7"/>
+      <c r="D151" s="8"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D152" s="7"/>
+      <c r="D152" s="8"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D153" s="7"/>
+      <c r="D153" s="8"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D154" s="7"/>
+      <c r="D154" s="8"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="7"/>
+      <c r="D155" s="8"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D156" s="7"/>
+      <c r="D156" s="8"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D157" s="7"/>
+      <c r="D157" s="8"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D158" s="7"/>
+      <c r="D158" s="8"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D159" s="7"/>
+      <c r="D159" s="8"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D160" s="7"/>
+      <c r="D160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D161" s="7"/>
+      <c r="D161" s="8"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D162" s="7"/>
+      <c r="D162" s="8"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="7"/>
+      <c r="D163" s="8"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D164" s="7"/>
+      <c r="D164" s="8"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D165" s="7"/>
+      <c r="D165" s="8"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D166" s="7"/>
+      <c r="D166" s="8"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D167" s="7"/>
+      <c r="D167" s="8"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="7"/>
+      <c r="D168" s="8"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D169" s="7"/>
+      <c r="D169" s="8"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D170" s="7"/>
+      <c r="D170" s="8"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D171" s="7"/>
+      <c r="D171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D172" s="7"/>
+      <c r="D172" s="8"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D173" s="7"/>
+      <c r="D173" s="8"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D174" s="7"/>
+      <c r="D174" s="8"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D175" s="7"/>
+      <c r="D175" s="8"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D176" s="7"/>
+      <c r="D176" s="8"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D177" s="7"/>
+      <c r="D177" s="8"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D178" s="7"/>
+      <c r="D178" s="8"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D179" s="7"/>
+      <c r="D179" s="8"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D180" s="7"/>
+      <c r="D180" s="8"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D181" s="7"/>
+      <c r="D181" s="8"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D182" s="7"/>
+      <c r="D182" s="8"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D183" s="7"/>
+      <c r="D183" s="8"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D184" s="7"/>
+      <c r="D184" s="8"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D185" s="7"/>
+      <c r="D185" s="8"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D186" s="7"/>
+      <c r="D186" s="8"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D187" s="7"/>
+      <c r="D187" s="8"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D188" s="7"/>
+      <c r="D188" s="8"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D189" s="7"/>
+      <c r="D189" s="8"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D190" s="7"/>
+      <c r="D190" s="8"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D191" s="7"/>
+      <c r="D191" s="8"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D192" s="7"/>
+      <c r="D192" s="8"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D193" s="7"/>
+      <c r="D193" s="8"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D194" s="7"/>
+      <c r="D194" s="8"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D195" s="7"/>
+      <c r="D195" s="8"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D196" s="7"/>
+      <c r="D196" s="8"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D197" s="7"/>
+      <c r="D197" s="8"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D198" s="7"/>
+      <c r="D198" s="8"/>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D199" s="7"/>
+      <c r="D199" s="8"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D200" s="7"/>
+      <c r="D200" s="8"/>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D201" s="7"/>
+      <c r="D201" s="8"/>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D202" s="7"/>
+      <c r="D202" s="8"/>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D203" s="7"/>
+      <c r="D203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D204" s="7"/>
+      <c r="D204" s="8"/>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D205" s="7"/>
+      <c r="D205" s="8"/>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D206" s="7"/>
+      <c r="D206" s="8"/>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D207" s="7"/>
+      <c r="D207" s="8"/>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D208" s="7"/>
+      <c r="D208" s="8"/>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D209" s="7"/>
+      <c r="D209" s="8"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D210" s="7"/>
+      <c r="D210" s="8"/>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D211" s="7"/>
+      <c r="D211" s="8"/>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D212" s="7"/>
+      <c r="D212" s="8"/>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D213" s="7"/>
+      <c r="D213" s="8"/>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D214" s="7"/>
+      <c r="D214" s="8"/>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D215" s="7"/>
+      <c r="D215" s="8"/>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D216" s="7"/>
+      <c r="D216" s="8"/>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D217" s="7"/>
+      <c r="D217" s="8"/>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D218" s="7"/>
+      <c r="D218" s="8"/>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D219" s="7"/>
+      <c r="D219" s="8"/>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D220" s="7"/>
+      <c r="D220" s="8"/>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D221" s="7"/>
+      <c r="D221" s="8"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D222" s="7"/>
+      <c r="D222" s="8"/>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D223" s="7"/>
+      <c r="D223" s="8"/>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D224" s="7"/>
+      <c r="D224" s="8"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D225" s="7"/>
+      <c r="D225" s="8"/>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D226" s="7"/>
+      <c r="D226" s="8"/>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D227" s="7"/>
+      <c r="D227" s="8"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D228" s="7"/>
+      <c r="D228" s="8"/>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D229" s="7"/>
+      <c r="D229" s="8"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D230" s="7"/>
+      <c r="D230" s="8"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D231" s="7"/>
+      <c r="D231" s="8"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D232" s="7"/>
+      <c r="D232" s="8"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D233" s="7"/>
+      <c r="D233" s="8"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D234" s="7"/>
+      <c r="D234" s="8"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D235" s="7"/>
+      <c r="D235" s="8"/>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D236" s="7"/>
+      <c r="D236" s="8"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D237" s="7"/>
+      <c r="D237" s="8"/>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D238" s="7"/>
+      <c r="D238" s="8"/>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D239" s="7"/>
+      <c r="D239" s="8"/>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D240" s="7"/>
+      <c r="D240" s="8"/>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D241" s="7"/>
+      <c r="D241" s="8"/>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D242" s="7"/>
+      <c r="D242" s="8"/>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D243" s="7"/>
+      <c r="D243" s="8"/>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D244" s="7"/>
+      <c r="D244" s="8"/>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D245" s="7"/>
+      <c r="D245" s="8"/>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D246" s="7"/>
+      <c r="D246" s="8"/>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D247" s="7"/>
+      <c r="D247" s="8"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D248" s="7"/>
+      <c r="D248" s="8"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D249" s="7"/>
+      <c r="D249" s="8"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D250" s="7"/>
+      <c r="D250" s="8"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D251" s="7"/>
+      <c r="D251" s="8"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D252" s="7"/>
+      <c r="D252" s="8"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D253" s="7"/>
+      <c r="D253" s="8"/>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D254" s="7"/>
+      <c r="D254" s="8"/>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D255" s="7"/>
+      <c r="D255" s="8"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D256" s="7"/>
+      <c r="D256" s="8"/>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D257" s="7"/>
+      <c r="D257" s="8"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D258" s="7"/>
+      <c r="D258" s="8"/>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D259" s="7"/>
+      <c r="D259" s="8"/>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D260" s="7"/>
+      <c r="D260" s="8"/>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D261" s="7"/>
+      <c r="D261" s="8"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D262" s="7"/>
+      <c r="D262" s="8"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D263" s="7"/>
+      <c r="D263" s="8"/>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D264" s="7"/>
+      <c r="D264" s="8"/>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D265" s="7"/>
+      <c r="D265" s="8"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D266" s="7"/>
+      <c r="D266" s="8"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D267" s="7"/>
+      <c r="D267" s="8"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D268" s="7"/>
+      <c r="D268" s="8"/>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D269" s="7"/>
+      <c r="D269" s="8"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D270" s="7"/>
+      <c r="D270" s="8"/>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D271" s="7"/>
+      <c r="D271" s="8"/>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D272" s="7"/>
+      <c r="D272" s="8"/>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D273" s="7"/>
+      <c r="D273" s="8"/>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D274" s="7"/>
+      <c r="D274" s="8"/>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D275" s="7"/>
+      <c r="D275" s="8"/>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D276" s="7"/>
+      <c r="D276" s="8"/>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D277" s="7"/>
+      <c r="D277" s="8"/>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D278" s="7"/>
+      <c r="D278" s="8"/>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D279" s="7"/>
+      <c r="D279" s="8"/>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D280" s="7"/>
+      <c r="D280" s="8"/>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D281" s="7"/>
+      <c r="D281" s="8"/>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D282" s="7"/>
+      <c r="D282" s="8"/>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D283" s="7"/>
+      <c r="D283" s="8"/>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D284" s="7"/>
+      <c r="D284" s="8"/>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D285" s="7"/>
+      <c r="D285" s="8"/>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D286" s="7"/>
+      <c r="D286" s="8"/>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D287" s="7"/>
+      <c r="D287" s="8"/>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D288" s="7"/>
+      <c r="D288" s="8"/>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D289" s="7"/>
+      <c r="D289" s="8"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D290" s="7"/>
+      <c r="D290" s="8"/>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D291" s="7"/>
+      <c r="D291" s="8"/>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D292" s="7"/>
+      <c r="D292" s="8"/>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D293" s="7"/>
+      <c r="D293" s="8"/>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D294" s="7"/>
+      <c r="D294" s="8"/>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D295" s="7"/>
+      <c r="D295" s="8"/>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D296" s="7"/>
+      <c r="D296" s="8"/>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D297" s="7"/>
+      <c r="D297" s="8"/>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D298" s="7"/>
+      <c r="D298" s="8"/>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D299" s="7"/>
+      <c r="D299" s="8"/>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D300" s="7"/>
+      <c r="D300" s="8"/>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D301" s="7"/>
+      <c r="D301" s="8"/>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D302" s="7"/>
+      <c r="D302" s="8"/>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D303" s="7"/>
+      <c r="D303" s="8"/>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D304" s="7"/>
+      <c r="D304" s="8"/>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D305" s="7"/>
+      <c r="D305" s="8"/>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D306" s="7"/>
+      <c r="D306" s="8"/>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D307" s="7"/>
+      <c r="D307" s="8"/>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D308" s="7"/>
+      <c r="D308" s="8"/>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D309" s="7"/>
+      <c r="D309" s="8"/>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D310" s="7"/>
+      <c r="D310" s="8"/>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D311" s="7"/>
+      <c r="D311" s="8"/>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D312" s="7"/>
+      <c r="D312" s="8"/>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D313" s="7"/>
+      <c r="D313" s="8"/>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D314" s="7"/>
+      <c r="D314" s="8"/>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D315" s="7"/>
+      <c r="D315" s="8"/>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D316" s="7"/>
+      <c r="D316" s="8"/>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D317" s="7"/>
+      <c r="D317" s="8"/>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D318" s="7"/>
+      <c r="D318" s="8"/>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D319" s="7"/>
+      <c r="D319" s="8"/>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D320" s="7"/>
+      <c r="D320" s="8"/>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D321" s="7"/>
+      <c r="D321" s="8"/>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D322" s="7"/>
+      <c r="D322" s="8"/>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D323" s="7"/>
+      <c r="D323" s="8"/>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D324" s="7"/>
+      <c r="D324" s="8"/>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D325" s="7"/>
+      <c r="D325" s="8"/>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D326" s="7"/>
+      <c r="D326" s="8"/>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D327" s="7"/>
+      <c r="D327" s="8"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D328" s="7"/>
+      <c r="D328" s="8"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D329" s="7"/>
+      <c r="D329" s="8"/>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D330" s="7"/>
+      <c r="D330" s="8"/>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D331" s="7"/>
+      <c r="D331" s="8"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D332" s="7"/>
+      <c r="D332" s="8"/>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D333" s="7"/>
+      <c r="D333" s="8"/>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D334" s="7"/>
+      <c r="D334" s="8"/>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D335" s="7"/>
+      <c r="D335" s="8"/>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D336" s="7"/>
+      <c r="D336" s="8"/>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D337" s="7"/>
+      <c r="D337" s="8"/>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D338" s="7"/>
+      <c r="D338" s="8"/>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D339" s="7"/>
+      <c r="D339" s="8"/>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D340" s="7"/>
+      <c r="D340" s="8"/>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D341" s="7"/>
+      <c r="D341" s="8"/>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D342" s="7"/>
+      <c r="D342" s="8"/>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D343" s="7"/>
+      <c r="D343" s="8"/>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D344" s="7"/>
+      <c r="D344" s="8"/>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D345" s="7"/>
+      <c r="D345" s="8"/>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D346" s="7"/>
+      <c r="D346" s="8"/>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D347" s="7"/>
+      <c r="D347" s="8"/>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D348" s="7"/>
+      <c r="D348" s="8"/>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D349" s="7"/>
+      <c r="D349" s="8"/>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D350" s="7"/>
+      <c r="D350" s="8"/>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D351" s="7"/>
+      <c r="D351" s="8"/>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D352" s="7"/>
+      <c r="D352" s="8"/>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D353" s="7"/>
+      <c r="D353" s="8"/>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D354" s="7"/>
+      <c r="D354" s="8"/>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D355" s="7"/>
+      <c r="D355" s="8"/>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D356" s="7"/>
+      <c r="D356" s="8"/>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D357" s="7"/>
+      <c r="D357" s="8"/>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D358" s="7"/>
+      <c r="D358" s="8"/>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D359" s="7"/>
+      <c r="D359" s="8"/>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D360" s="7"/>
+      <c r="D360" s="8"/>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D361" s="7"/>
+      <c r="D361" s="8"/>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D362" s="7"/>
+      <c r="D362" s="8"/>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D363" s="7"/>
+      <c r="D363" s="8"/>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D364" s="7"/>
+      <c r="D364" s="8"/>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D365" s="7"/>
+      <c r="D365" s="8"/>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D366" s="7"/>
+      <c r="D366" s="8"/>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D367" s="7"/>
+      <c r="D367" s="8"/>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D368" s="7"/>
+      <c r="D368" s="8"/>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D369" s="7"/>
+      <c r="D369" s="8"/>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D370" s="7"/>
+      <c r="D370" s="8"/>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D371" s="7"/>
+      <c r="D371" s="8"/>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D372" s="7"/>
+      <c r="D372" s="8"/>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D373" s="7"/>
+      <c r="D373" s="8"/>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D374" s="7"/>
+      <c r="D374" s="8"/>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D375" s="7"/>
+      <c r="D375" s="8"/>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D376" s="7"/>
+      <c r="D376" s="8"/>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D377" s="7"/>
+      <c r="D377" s="8"/>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D378" s="7"/>
+      <c r="D378" s="8"/>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D379" s="7"/>
+      <c r="D379" s="8"/>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D380" s="7"/>
+      <c r="D380" s="8"/>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D381" s="7"/>
+      <c r="D381" s="8"/>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D382" s="7"/>
+      <c r="D382" s="8"/>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D383" s="7"/>
+      <c r="D383" s="8"/>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D384" s="7"/>
+      <c r="D384" s="8"/>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D385" s="7"/>
+      <c r="D385" s="8"/>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D386" s="7"/>
+      <c r="D386" s="8"/>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D387" s="7"/>
+      <c r="D387" s="8"/>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D388" s="7"/>
+      <c r="D388" s="8"/>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D389" s="7"/>
+      <c r="D389" s="8"/>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D390" s="7"/>
+      <c r="D390" s="8"/>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D391" s="7"/>
+      <c r="D391" s="8"/>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D392" s="7"/>
+      <c r="D392" s="8"/>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D393" s="7"/>
+      <c r="D393" s="8"/>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D394" s="7"/>
+      <c r="D394" s="8"/>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D395" s="7"/>
+      <c r="D395" s="8"/>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D396" s="7"/>
+      <c r="D396" s="8"/>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D397" s="7"/>
+      <c r="D397" s="8"/>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D398" s="7"/>
+      <c r="D398" s="8"/>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D399" s="7"/>
+      <c r="D399" s="8"/>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D400" s="7"/>
+      <c r="D400" s="8"/>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D401" s="7"/>
+      <c r="D401" s="8"/>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D402" s="7"/>
+      <c r="D402" s="8"/>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D403" s="7"/>
+      <c r="D403" s="8"/>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D404" s="7"/>
+      <c r="D404" s="8"/>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D405" s="7"/>
+      <c r="D405" s="8"/>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D406" s="7"/>
+      <c r="D406" s="8"/>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D407" s="7"/>
+      <c r="D407" s="8"/>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D408" s="7"/>
+      <c r="D408" s="8"/>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D409" s="7"/>
+      <c r="D409" s="8"/>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D410" s="7"/>
+      <c r="D410" s="8"/>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D411" s="7"/>
+      <c r="D411" s="8"/>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D412" s="7"/>
+      <c r="D412" s="8"/>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D413" s="7"/>
+      <c r="D413" s="8"/>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D414" s="7"/>
+      <c r="D414" s="8"/>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D415" s="7"/>
+      <c r="D415" s="8"/>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D416" s="7"/>
+      <c r="D416" s="8"/>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D417" s="7"/>
+      <c r="D417" s="8"/>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D418" s="7"/>
+      <c r="D418" s="8"/>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D419" s="7"/>
+      <c r="D419" s="8"/>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D420" s="7"/>
+      <c r="D420" s="8"/>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D421" s="7"/>
+      <c r="D421" s="8"/>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D422" s="7"/>
+      <c r="D422" s="8"/>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D423" s="7"/>
+      <c r="D423" s="8"/>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D424" s="7"/>
+      <c r="D424" s="8"/>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D425" s="7"/>
+      <c r="D425" s="8"/>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D426" s="7"/>
+      <c r="D426" s="8"/>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D427" s="7"/>
+      <c r="D427" s="8"/>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D428" s="7"/>
+      <c r="D428" s="8"/>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D429" s="7"/>
+      <c r="D429" s="8"/>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D430" s="7"/>
+      <c r="D430" s="8"/>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D431" s="7"/>
+      <c r="D431" s="8"/>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D432" s="7"/>
+      <c r="D432" s="8"/>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D433" s="7"/>
+      <c r="D433" s="8"/>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D434" s="7"/>
+      <c r="D434" s="8"/>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D435" s="7"/>
+      <c r="D435" s="8"/>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D436" s="7"/>
+      <c r="D436" s="8"/>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D437" s="7"/>
+      <c r="D437" s="8"/>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D438" s="7"/>
+      <c r="D438" s="8"/>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D439" s="7"/>
+      <c r="D439" s="8"/>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D440" s="7"/>
+      <c r="D440" s="8"/>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D441" s="7"/>
+      <c r="D441" s="8"/>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D442" s="7"/>
+      <c r="D442" s="8"/>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D443" s="7"/>
+      <c r="D443" s="8"/>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D444" s="7"/>
+      <c r="D444" s="8"/>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D445" s="7"/>
+      <c r="D445" s="8"/>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D446" s="7"/>
+      <c r="D446" s="8"/>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D447" s="7"/>
+      <c r="D447" s="8"/>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D448" s="7"/>
+      <c r="D448" s="8"/>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D449" s="7"/>
+      <c r="D449" s="8"/>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D450" s="7"/>
+      <c r="D450" s="8"/>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D451" s="7"/>
+      <c r="D451" s="8"/>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D452" s="7"/>
+      <c r="D452" s="8"/>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D453" s="7"/>
+      <c r="D453" s="8"/>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D454" s="7"/>
+      <c r="D454" s="8"/>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D455" s="7"/>
+      <c r="D455" s="8"/>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D456" s="7"/>
+      <c r="D456" s="8"/>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D457" s="7"/>
+      <c r="D457" s="8"/>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D458" s="7"/>
+      <c r="D458" s="8"/>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D459" s="7"/>
+      <c r="D459" s="8"/>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D460" s="7"/>
+      <c r="D460" s="8"/>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D461" s="7"/>
+      <c r="D461" s="8"/>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D462" s="7"/>
+      <c r="D462" s="8"/>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D463" s="7"/>
+      <c r="D463" s="8"/>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D464" s="7"/>
+      <c r="D464" s="8"/>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D465" s="7"/>
+      <c r="D465" s="8"/>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D466" s="7"/>
+      <c r="D466" s="8"/>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D467" s="7"/>
+      <c r="D467" s="8"/>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D468" s="7"/>
+      <c r="D468" s="8"/>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D469" s="7"/>
+      <c r="D469" s="8"/>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D470" s="7"/>
+      <c r="D470" s="8"/>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D471" s="7"/>
+      <c r="D471" s="8"/>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D472" s="7"/>
+      <c r="D472" s="8"/>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D473" s="7"/>
+      <c r="D473" s="8"/>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D474" s="7"/>
+      <c r="D474" s="8"/>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D475" s="7"/>
+      <c r="D475" s="8"/>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D476" s="7"/>
+      <c r="D476" s="8"/>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D477" s="7"/>
+      <c r="D477" s="8"/>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D478" s="7"/>
+      <c r="D478" s="8"/>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D479" s="7"/>
+      <c r="D479" s="8"/>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D480" s="7"/>
+      <c r="D480" s="8"/>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D481" s="7"/>
+      <c r="D481" s="8"/>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D482" s="7"/>
+      <c r="D482" s="8"/>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D483" s="7"/>
+      <c r="D483" s="8"/>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D484" s="7"/>
+      <c r="D484" s="8"/>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D485" s="7"/>
+      <c r="D485" s="8"/>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D486" s="7"/>
+      <c r="D486" s="8"/>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D487" s="7"/>
+      <c r="D487" s="8"/>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D488" s="7"/>
+      <c r="D488" s="8"/>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D489" s="7"/>
+      <c r="D489" s="8"/>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D490" s="7"/>
+      <c r="D490" s="8"/>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D491" s="7"/>
+      <c r="D491" s="8"/>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D492" s="7"/>
+      <c r="D492" s="8"/>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D493" s="7"/>
+      <c r="D493" s="8"/>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D494" s="7"/>
+      <c r="D494" s="8"/>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D495" s="7"/>
+      <c r="D495" s="8"/>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D496" s="7"/>
+      <c r="D496" s="8"/>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D497" s="7"/>
+      <c r="D497" s="8"/>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D498" s="7"/>
+      <c r="D498" s="8"/>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D499" s="7"/>
+      <c r="D499" s="8"/>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D500" s="7"/>
+      <c r="D500" s="8"/>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D501" s="7"/>
+      <c r="D501" s="8"/>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D502" s="7"/>
+      <c r="D502" s="8"/>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D503" s="7"/>
+      <c r="D503" s="8"/>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D504" s="7"/>
+      <c r="D504" s="8"/>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D505" s="7"/>
+      <c r="D505" s="8"/>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D506" s="7"/>
+      <c r="D506" s="8"/>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D507" s="7"/>
+      <c r="D507" s="8"/>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D508" s="7"/>
+      <c r="D508" s="8"/>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D509" s="7"/>
+      <c r="D509" s="8"/>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D510" s="7"/>
+      <c r="D510" s="8"/>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D511" s="7"/>
+      <c r="D511" s="8"/>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D512" s="7"/>
+      <c r="D512" s="8"/>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D513" s="7"/>
+      <c r="D513" s="8"/>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D514" s="7"/>
+      <c r="D514" s="8"/>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D515" s="7"/>
+      <c r="D515" s="8"/>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D516" s="7"/>
+      <c r="D516" s="8"/>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D517" s="7"/>
+      <c r="D517" s="8"/>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D518" s="7"/>
+      <c r="D518" s="8"/>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D519" s="7"/>
+      <c r="D519" s="8"/>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D520" s="7"/>
+      <c r="D520" s="8"/>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D521" s="7"/>
+      <c r="D521" s="8"/>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D522" s="7"/>
+      <c r="D522" s="8"/>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D523" s="7"/>
+      <c r="D523" s="8"/>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D524" s="7"/>
+      <c r="D524" s="8"/>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D525" s="7"/>
+      <c r="D525" s="8"/>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D526" s="7"/>
+      <c r="D526" s="8"/>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D527" s="7"/>
+      <c r="D527" s="8"/>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D528" s="7"/>
+      <c r="D528" s="8"/>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D529" s="7"/>
+      <c r="D529" s="8"/>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D530" s="7"/>
+      <c r="D530" s="8"/>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D531" s="7"/>
+      <c r="D531" s="8"/>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D532" s="7"/>
+      <c r="D532" s="8"/>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D533" s="7"/>
+      <c r="D533" s="8"/>
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D534" s="7"/>
+      <c r="D534" s="8"/>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D535" s="7"/>
+      <c r="D535" s="8"/>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D536" s="7"/>
+      <c r="D536" s="8"/>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D537" s="7"/>
+      <c r="D537" s="8"/>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D538" s="7"/>
+      <c r="D538" s="8"/>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D539" s="7"/>
+      <c r="D539" s="8"/>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D540" s="7"/>
+      <c r="D540" s="8"/>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D541" s="7"/>
+      <c r="D541" s="8"/>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D542" s="7"/>
+      <c r="D542" s="8"/>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D543" s="7"/>
+      <c r="D543" s="8"/>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D544" s="7"/>
+      <c r="D544" s="8"/>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D545" s="7"/>
+      <c r="D545" s="8"/>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D546" s="7"/>
+      <c r="D546" s="8"/>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D547" s="7"/>
+      <c r="D547" s="8"/>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D548" s="7"/>
+      <c r="D548" s="8"/>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D549" s="7"/>
+      <c r="D549" s="8"/>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D550" s="7"/>
+      <c r="D550" s="8"/>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D551" s="7"/>
+      <c r="D551" s="8"/>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D552" s="7"/>
+      <c r="D552" s="8"/>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D553" s="7"/>
+      <c r="D553" s="8"/>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D554" s="7"/>
+      <c r="D554" s="8"/>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D555" s="7"/>
+      <c r="D555" s="8"/>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D556" s="7"/>
+      <c r="D556" s="8"/>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D557" s="7"/>
+      <c r="D557" s="8"/>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D558" s="7"/>
+      <c r="D558" s="8"/>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D559" s="7"/>
+      <c r="D559" s="8"/>
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D560" s="7"/>
+      <c r="D560" s="8"/>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D561" s="7"/>
+      <c r="D561" s="8"/>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D562" s="7"/>
+      <c r="D562" s="8"/>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D563" s="7"/>
+      <c r="D563" s="8"/>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D564" s="7"/>
+      <c r="D564" s="8"/>
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D565" s="7"/>
+      <c r="D565" s="8"/>
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D566" s="7"/>
+      <c r="D566" s="8"/>
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D567" s="7"/>
+      <c r="D567" s="8"/>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D568" s="7"/>
+      <c r="D568" s="8"/>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D569" s="7"/>
+      <c r="D569" s="8"/>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D570" s="7"/>
+      <c r="D570" s="8"/>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D571" s="7"/>
+      <c r="D571" s="8"/>
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D572" s="7"/>
+      <c r="D572" s="8"/>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D573" s="7"/>
+      <c r="D573" s="8"/>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D574" s="7"/>
+      <c r="D574" s="8"/>
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D575" s="7"/>
+      <c r="D575" s="8"/>
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D576" s="7"/>
+      <c r="D576" s="8"/>
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D577" s="7"/>
+      <c r="D577" s="8"/>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D578" s="7"/>
+      <c r="D578" s="8"/>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D579" s="7"/>
+      <c r="D579" s="8"/>
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D580" s="7"/>
+      <c r="D580" s="8"/>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D581" s="7"/>
+      <c r="D581" s="8"/>
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D582" s="7"/>
+      <c r="D582" s="8"/>
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D583" s="7"/>
+      <c r="D583" s="8"/>
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D584" s="7"/>
+      <c r="D584" s="8"/>
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D585" s="7"/>
+      <c r="D585" s="8"/>
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D586" s="7"/>
+      <c r="D586" s="8"/>
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D587" s="7"/>
+      <c r="D587" s="8"/>
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D588" s="7"/>
+      <c r="D588" s="8"/>
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D589" s="7"/>
+      <c r="D589" s="8"/>
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D590" s="7"/>
+      <c r="D590" s="8"/>
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D591" s="7"/>
+      <c r="D591" s="8"/>
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D592" s="7"/>
+      <c r="D592" s="8"/>
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D593" s="7"/>
+      <c r="D593" s="8"/>
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D594" s="7"/>
+      <c r="D594" s="8"/>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D595" s="7"/>
+      <c r="D595" s="8"/>
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D596" s="7"/>
+      <c r="D596" s="8"/>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D597" s="7"/>
+      <c r="D597" s="8"/>
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D598" s="7"/>
+      <c r="D598" s="8"/>
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D599" s="7"/>
+      <c r="D599" s="8"/>
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D600" s="7"/>
+      <c r="D600" s="8"/>
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D601" s="7"/>
+      <c r="D601" s="8"/>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D602" s="7"/>
+      <c r="D602" s="8"/>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D603" s="7"/>
+      <c r="D603" s="8"/>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D604" s="7"/>
+      <c r="D604" s="8"/>
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D605" s="7"/>
+      <c r="D605" s="8"/>
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D606" s="7"/>
+      <c r="D606" s="8"/>
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D607" s="7"/>
+      <c r="D607" s="8"/>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D608" s="7"/>
+      <c r="D608" s="8"/>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D609" s="7"/>
+      <c r="D609" s="8"/>
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D610" s="7"/>
+      <c r="D610" s="8"/>
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D611" s="7"/>
+      <c r="D611" s="8"/>
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D612" s="7"/>
+      <c r="D612" s="8"/>
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D613" s="7"/>
+      <c r="D613" s="8"/>
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D614" s="7"/>
+      <c r="D614" s="8"/>
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D615" s="7"/>
+      <c r="D615" s="8"/>
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D616" s="7"/>
+      <c r="D616" s="8"/>
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D617" s="7"/>
+      <c r="D617" s="8"/>
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D618" s="7"/>
+      <c r="D618" s="8"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D619" s="7"/>
+      <c r="D619" s="8"/>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D620" s="7"/>
+      <c r="D620" s="8"/>
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D621" s="7"/>
+      <c r="D621" s="8"/>
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D622" s="7"/>
+      <c r="D622" s="8"/>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D623" s="7"/>
+      <c r="D623" s="8"/>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D624" s="7"/>
+      <c r="D624" s="8"/>
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D625" s="7"/>
+      <c r="D625" s="8"/>
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D626" s="7"/>
+      <c r="D626" s="8"/>
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D627" s="7"/>
+      <c r="D627" s="8"/>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D628" s="7"/>
+      <c r="D628" s="8"/>
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D629" s="7"/>
+      <c r="D629" s="8"/>
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D630" s="7"/>
+      <c r="D630" s="8"/>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D631" s="7"/>
+      <c r="D631" s="8"/>
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D632" s="7"/>
+      <c r="D632" s="8"/>
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D633" s="7"/>
+      <c r="D633" s="8"/>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D634" s="7"/>
+      <c r="D634" s="8"/>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D635" s="7"/>
+      <c r="D635" s="8"/>
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D636" s="7"/>
+      <c r="D636" s="8"/>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D637" s="7"/>
+      <c r="D637" s="8"/>
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D638" s="7"/>
+      <c r="D638" s="8"/>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D639" s="7"/>
+      <c r="D639" s="8"/>
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D640" s="7"/>
+      <c r="D640" s="8"/>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D641" s="7"/>
+      <c r="D641" s="8"/>
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D642" s="7"/>
+      <c r="D642" s="8"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D643" s="7"/>
+      <c r="D643" s="8"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D644" s="7"/>
+      <c r="D644" s="8"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D645" s="7"/>
+      <c r="D645" s="8"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D646" s="7"/>
+      <c r="D646" s="8"/>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D647" s="7"/>
+      <c r="D647" s="8"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D648" s="7"/>
+      <c r="D648" s="8"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D649" s="7"/>
+      <c r="D649" s="8"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D650" s="7"/>
+      <c r="D650" s="8"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D651" s="7"/>
+      <c r="D651" s="8"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D652" s="7"/>
+      <c r="D652" s="8"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D653" s="7"/>
+      <c r="D653" s="8"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D654" s="7"/>
+      <c r="D654" s="8"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D655" s="7"/>
+      <c r="D655" s="8"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D656" s="7"/>
+      <c r="D656" s="8"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D657" s="7"/>
+      <c r="D657" s="8"/>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D658" s="7"/>
+      <c r="D658" s="8"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D659" s="7"/>
+      <c r="D659" s="8"/>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D660" s="7"/>
+      <c r="D660" s="8"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D661" s="7"/>
+      <c r="D661" s="8"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D662" s="7"/>
+      <c r="D662" s="8"/>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D663" s="7"/>
+      <c r="D663" s="8"/>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D664" s="7"/>
+      <c r="D664" s="8"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D665" s="7"/>
+      <c r="D665" s="8"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D666" s="7"/>
+      <c r="D666" s="8"/>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D667" s="7"/>
+      <c r="D667" s="8"/>
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D668" s="7"/>
+      <c r="D668" s="8"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D669" s="7"/>
+      <c r="D669" s="8"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D670" s="7"/>
+      <c r="D670" s="8"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D671" s="7"/>
+      <c r="D671" s="8"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D672" s="7"/>
+      <c r="D672" s="8"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D673" s="7"/>
+      <c r="D673" s="8"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D674" s="7"/>
+      <c r="D674" s="8"/>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D675" s="7"/>
+      <c r="D675" s="8"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D676" s="7"/>
+      <c r="D676" s="8"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D677" s="7"/>
+      <c r="D677" s="8"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D678" s="7"/>
+      <c r="D678" s="8"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D679" s="7"/>
+      <c r="D679" s="8"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D680" s="7"/>
+      <c r="D680" s="8"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D681" s="7"/>
+      <c r="D681" s="8"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D682" s="7"/>
+      <c r="D682" s="8"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D683" s="7"/>
+      <c r="D683" s="8"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D684" s="7"/>
+      <c r="D684" s="8"/>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D685" s="7"/>
+      <c r="D685" s="8"/>
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D686" s="7"/>
+      <c r="D686" s="8"/>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D687" s="7"/>
+      <c r="D687" s="8"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D688" s="7"/>
+      <c r="D688" s="8"/>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D689" s="7"/>
+      <c r="D689" s="8"/>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D690" s="7"/>
+      <c r="D690" s="8"/>
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D691" s="7"/>
+      <c r="D691" s="8"/>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D692" s="7"/>
+      <c r="D692" s="8"/>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D693" s="7"/>
+      <c r="D693" s="8"/>
     </row>
     <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D694" s="7"/>
+      <c r="D694" s="8"/>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D695" s="7"/>
+      <c r="D695" s="8"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D696" s="7"/>
+      <c r="D696" s="8"/>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D697" s="7"/>
+      <c r="D697" s="8"/>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D698" s="7"/>
+      <c r="D698" s="8"/>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D699" s="7"/>
+      <c r="D699" s="8"/>
     </row>
     <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D700" s="7"/>
+      <c r="D700" s="8"/>
     </row>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D701" s="7"/>
+      <c r="D701" s="8"/>
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D702" s="7"/>
+      <c r="D702" s="8"/>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D703" s="7"/>
+      <c r="D703" s="8"/>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D704" s="7"/>
+      <c r="D704" s="8"/>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D705" s="7"/>
+      <c r="D705" s="8"/>
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D706" s="7"/>
+      <c r="D706" s="8"/>
     </row>
     <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D707" s="7"/>
+      <c r="D707" s="8"/>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D708" s="7"/>
+      <c r="D708" s="8"/>
     </row>
     <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D709" s="7"/>
+      <c r="D709" s="8"/>
     </row>
     <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D710" s="7"/>
+      <c r="D710" s="8"/>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D711" s="7"/>
+      <c r="D711" s="8"/>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D712" s="7"/>
+      <c r="D712" s="8"/>
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D713" s="7"/>
+      <c r="D713" s="8"/>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D714" s="7"/>
+      <c r="D714" s="8"/>
     </row>
     <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D715" s="7"/>
+      <c r="D715" s="8"/>
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D716" s="7"/>
+      <c r="D716" s="8"/>
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D717" s="7"/>
+      <c r="D717" s="8"/>
     </row>
     <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D718" s="7"/>
+      <c r="D718" s="8"/>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D719" s="7"/>
+      <c r="D719" s="8"/>
     </row>
     <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D720" s="7"/>
+      <c r="D720" s="8"/>
     </row>
     <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D721" s="7"/>
+      <c r="D721" s="8"/>
     </row>
     <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D722" s="7"/>
+      <c r="D722" s="8"/>
     </row>
     <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D723" s="7"/>
+      <c r="D723" s="8"/>
     </row>
     <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D724" s="7"/>
+      <c r="D724" s="8"/>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D725" s="7"/>
+      <c r="D725" s="8"/>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D726" s="7"/>
+      <c r="D726" s="8"/>
     </row>
     <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D727" s="7"/>
+      <c r="D727" s="8"/>
     </row>
     <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D728" s="7"/>
+      <c r="D728" s="8"/>
     </row>
     <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D729" s="7"/>
+      <c r="D729" s="8"/>
     </row>
     <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D730" s="7"/>
+      <c r="D730" s="8"/>
     </row>
     <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D731" s="7"/>
+      <c r="D731" s="8"/>
     </row>
     <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D732" s="7"/>
+      <c r="D732" s="8"/>
     </row>
     <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D733" s="7"/>
+      <c r="D733" s="8"/>
     </row>
     <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D734" s="7"/>
+      <c r="D734" s="8"/>
     </row>
     <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D735" s="7"/>
+      <c r="D735" s="8"/>
     </row>
     <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D736" s="7"/>
+      <c r="D736" s="8"/>
     </row>
     <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D737" s="7"/>
+      <c r="D737" s="8"/>
     </row>
     <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D738" s="7"/>
+      <c r="D738" s="8"/>
     </row>
     <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D739" s="7"/>
+      <c r="D739" s="8"/>
     </row>
     <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D740" s="7"/>
+      <c r="D740" s="8"/>
     </row>
     <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D741" s="7"/>
+      <c r="D741" s="8"/>
     </row>
     <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D742" s="7"/>
+      <c r="D742" s="8"/>
     </row>
     <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D743" s="7"/>
+      <c r="D743" s="8"/>
     </row>
     <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D744" s="7"/>
+      <c r="D744" s="8"/>
     </row>
     <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D745" s="7"/>
+      <c r="D745" s="8"/>
     </row>
     <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D746" s="7"/>
+      <c r="D746" s="8"/>
     </row>
     <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D747" s="7"/>
+      <c r="D747" s="8"/>
     </row>
     <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D748" s="7"/>
+      <c r="D748" s="8"/>
     </row>
     <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D749" s="7"/>
+      <c r="D749" s="8"/>
     </row>
     <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D750" s="7"/>
+      <c r="D750" s="8"/>
     </row>
     <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D751" s="7"/>
+      <c r="D751" s="8"/>
     </row>
     <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D752" s="7"/>
+      <c r="D752" s="8"/>
     </row>
     <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D753" s="7"/>
+      <c r="D753" s="8"/>
     </row>
     <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D754" s="7"/>
+      <c r="D754" s="8"/>
     </row>
     <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D755" s="7"/>
+      <c r="D755" s="8"/>
     </row>
     <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D756" s="7"/>
+      <c r="D756" s="8"/>
     </row>
     <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D757" s="7"/>
+      <c r="D757" s="8"/>
     </row>
     <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D758" s="7"/>
+      <c r="D758" s="8"/>
     </row>
     <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D759" s="7"/>
+      <c r="D759" s="8"/>
     </row>
     <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D760" s="7"/>
+      <c r="D760" s="8"/>
     </row>
     <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D761" s="7"/>
+      <c r="D761" s="8"/>
     </row>
     <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D762" s="7"/>
+      <c r="D762" s="8"/>
     </row>
     <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D763" s="7"/>
+      <c r="D763" s="8"/>
     </row>
     <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D764" s="7"/>
+      <c r="D764" s="8"/>
     </row>
     <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D765" s="7"/>
+      <c r="D765" s="8"/>
     </row>
     <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D766" s="7"/>
+      <c r="D766" s="8"/>
     </row>
     <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D767" s="7"/>
+      <c r="D767" s="8"/>
     </row>
     <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D768" s="7"/>
+      <c r="D768" s="8"/>
     </row>
     <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D769" s="7"/>
+      <c r="D769" s="8"/>
     </row>
     <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D770" s="7"/>
+      <c r="D770" s="8"/>
     </row>
     <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D771" s="7"/>
+      <c r="D771" s="8"/>
     </row>
     <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D772" s="7"/>
+      <c r="D772" s="8"/>
     </row>
     <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D773" s="7"/>
+      <c r="D773" s="8"/>
     </row>
     <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D774" s="7"/>
+      <c r="D774" s="8"/>
     </row>
     <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D775" s="7"/>
+      <c r="D775" s="8"/>
     </row>
     <row r="776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D776" s="7"/>
+      <c r="D776" s="8"/>
     </row>
     <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D777" s="7"/>
+      <c r="D777" s="8"/>
     </row>
     <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D778" s="7"/>
+      <c r="D778" s="8"/>
     </row>
     <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D779" s="7"/>
+      <c r="D779" s="8"/>
     </row>
     <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D780" s="7"/>
+      <c r="D780" s="8"/>
     </row>
     <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D781" s="7"/>
+      <c r="D781" s="8"/>
     </row>
     <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D782" s="7"/>
+      <c r="D782" s="8"/>
     </row>
     <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D783" s="7"/>
+      <c r="D783" s="8"/>
     </row>
     <row r="784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D784" s="7"/>
+      <c r="D784" s="8"/>
     </row>
     <row r="785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D785" s="7"/>
+      <c r="D785" s="8"/>
     </row>
     <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D786" s="7"/>
+      <c r="D786" s="8"/>
     </row>
     <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D787" s="7"/>
+      <c r="D787" s="8"/>
     </row>
     <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D788" s="7"/>
+      <c r="D788" s="8"/>
     </row>
     <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D789" s="7"/>
+      <c r="D789" s="8"/>
     </row>
     <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D790" s="7"/>
+      <c r="D790" s="8"/>
     </row>
     <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D791" s="7"/>
+      <c r="D791" s="8"/>
     </row>
     <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D792" s="7"/>
+      <c r="D792" s="8"/>
     </row>
     <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D793" s="7"/>
+      <c r="D793" s="8"/>
     </row>
     <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D794" s="7"/>
+      <c r="D794" s="8"/>
     </row>
     <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D795" s="7"/>
+      <c r="D795" s="8"/>
     </row>
     <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D796" s="7"/>
+      <c r="D796" s="8"/>
     </row>
     <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D797" s="7"/>
+      <c r="D797" s="8"/>
     </row>
     <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D798" s="7"/>
+      <c r="D798" s="8"/>
     </row>
     <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D799" s="7"/>
+      <c r="D799" s="8"/>
     </row>
     <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D800" s="7"/>
+      <c r="D800" s="8"/>
     </row>
     <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D801" s="7"/>
+      <c r="D801" s="8"/>
     </row>
     <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D802" s="7"/>
+      <c r="D802" s="8"/>
     </row>
     <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D803" s="7"/>
+      <c r="D803" s="8"/>
     </row>
     <row r="804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D804" s="7"/>
+      <c r="D804" s="8"/>
     </row>
     <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D805" s="7"/>
+      <c r="D805" s="8"/>
     </row>
     <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D806" s="7"/>
+      <c r="D806" s="8"/>
     </row>
     <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D807" s="7"/>
+      <c r="D807" s="8"/>
     </row>
     <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D808" s="7"/>
+      <c r="D808" s="8"/>
     </row>
     <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D809" s="7"/>
+      <c r="D809" s="8"/>
     </row>
     <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D810" s="7"/>
+      <c r="D810" s="8"/>
     </row>
     <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D811" s="7"/>
+      <c r="D811" s="8"/>
     </row>
     <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D812" s="7"/>
+      <c r="D812" s="8"/>
     </row>
     <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D813" s="7"/>
+      <c r="D813" s="8"/>
     </row>
     <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D814" s="7"/>
+      <c r="D814" s="8"/>
     </row>
     <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D815" s="7"/>
+      <c r="D815" s="8"/>
     </row>
     <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D816" s="7"/>
+      <c r="D816" s="8"/>
     </row>
     <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D817" s="7"/>
+      <c r="D817" s="8"/>
     </row>
     <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D818" s="7"/>
+      <c r="D818" s="8"/>
     </row>
     <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D819" s="7"/>
+      <c r="D819" s="8"/>
     </row>
     <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D820" s="7"/>
+      <c r="D820" s="8"/>
     </row>
     <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D821" s="7"/>
+      <c r="D821" s="8"/>
     </row>
     <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D822" s="7"/>
+      <c r="D822" s="8"/>
     </row>
     <row r="823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D823" s="7"/>
+      <c r="D823" s="8"/>
     </row>
     <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D824" s="7"/>
+      <c r="D824" s="8"/>
     </row>
     <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D825" s="7"/>
+      <c r="D825" s="8"/>
     </row>
     <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D826" s="7"/>
+      <c r="D826" s="8"/>
     </row>
     <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D827" s="7"/>
+      <c r="D827" s="8"/>
     </row>
     <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D828" s="7"/>
+      <c r="D828" s="8"/>
     </row>
     <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D829" s="7"/>
+      <c r="D829" s="8"/>
     </row>
     <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D830" s="7"/>
+      <c r="D830" s="8"/>
     </row>
     <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D831" s="7"/>
+      <c r="D831" s="8"/>
     </row>
     <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D832" s="7"/>
+      <c r="D832" s="8"/>
     </row>
     <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D833" s="7"/>
+      <c r="D833" s="8"/>
     </row>
     <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D834" s="7"/>
+      <c r="D834" s="8"/>
     </row>
     <row r="835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D835" s="7"/>
+      <c r="D835" s="8"/>
     </row>
     <row r="836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D836" s="7"/>
+      <c r="D836" s="8"/>
     </row>
     <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D837" s="7"/>
+      <c r="D837" s="8"/>
     </row>
     <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D838" s="7"/>
+      <c r="D838" s="8"/>
     </row>
     <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D839" s="7"/>
+      <c r="D839" s="8"/>
     </row>
     <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D840" s="7"/>
+      <c r="D840" s="8"/>
     </row>
     <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D841" s="7"/>
+      <c r="D841" s="8"/>
     </row>
     <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D842" s="7"/>
+      <c r="D842" s="8"/>
     </row>
     <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D843" s="7"/>
+      <c r="D843" s="8"/>
     </row>
     <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D844" s="7"/>
+      <c r="D844" s="8"/>
     </row>
     <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D845" s="7"/>
+      <c r="D845" s="8"/>
     </row>
     <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D846" s="7"/>
+      <c r="D846" s="8"/>
     </row>
     <row r="847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D847" s="7"/>
+      <c r="D847" s="8"/>
     </row>
     <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D848" s="7"/>
+      <c r="D848" s="8"/>
     </row>
     <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D849" s="7"/>
+      <c r="D849" s="8"/>
     </row>
     <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D850" s="7"/>
+      <c r="D850" s="8"/>
     </row>
     <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D851" s="7"/>
+      <c r="D851" s="8"/>
     </row>
     <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D852" s="7"/>
+      <c r="D852" s="8"/>
     </row>
     <row r="853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D853" s="7"/>
+      <c r="D853" s="8"/>
     </row>
     <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D854" s="7"/>
+      <c r="D854" s="8"/>
     </row>
     <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D855" s="7"/>
+      <c r="D855" s="8"/>
     </row>
     <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D856" s="7"/>
+      <c r="D856" s="8"/>
     </row>
     <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D857" s="7"/>
+      <c r="D857" s="8"/>
     </row>
     <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D858" s="7"/>
+      <c r="D858" s="8"/>
     </row>
     <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D859" s="7"/>
+      <c r="D859" s="8"/>
     </row>
     <row r="860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D860" s="7"/>
+      <c r="D860" s="8"/>
     </row>
     <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D861" s="7"/>
+      <c r="D861" s="8"/>
     </row>
     <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D862" s="7"/>
+      <c r="D862" s="8"/>
     </row>
     <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D863" s="7"/>
+      <c r="D863" s="8"/>
     </row>
     <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D864" s="7"/>
+      <c r="D864" s="8"/>
     </row>
     <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D865" s="7"/>
+      <c r="D865" s="8"/>
     </row>
     <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D866" s="7"/>
+      <c r="D866" s="8"/>
     </row>
     <row r="867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D867" s="7"/>
+      <c r="D867" s="8"/>
     </row>
     <row r="868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D868" s="7"/>
+      <c r="D868" s="8"/>
     </row>
     <row r="869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D869" s="7"/>
+      <c r="D869" s="8"/>
     </row>
     <row r="870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D870" s="7"/>
+      <c r="D870" s="8"/>
     </row>
     <row r="871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D871" s="7"/>
+      <c r="D871" s="8"/>
     </row>
     <row r="872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D872" s="7"/>
+      <c r="D872" s="8"/>
     </row>
     <row r="873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D873" s="7"/>
+      <c r="D873" s="8"/>
     </row>
     <row r="874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D874" s="7"/>
+      <c r="D874" s="8"/>
     </row>
     <row r="875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D875" s="7"/>
+      <c r="D875" s="8"/>
     </row>
     <row r="876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D876" s="7"/>
+      <c r="D876" s="8"/>
     </row>
     <row r="877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D877" s="7"/>
+      <c r="D877" s="8"/>
     </row>
     <row r="878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D878" s="7"/>
+      <c r="D878" s="8"/>
     </row>
     <row r="879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D879" s="7"/>
+      <c r="D879" s="8"/>
     </row>
     <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D880" s="7"/>
+      <c r="D880" s="8"/>
     </row>
     <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D881" s="7"/>
+      <c r="D881" s="8"/>
     </row>
     <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D882" s="7"/>
+      <c r="D882" s="8"/>
     </row>
     <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D883" s="7"/>
+      <c r="D883" s="8"/>
     </row>
     <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D884" s="7"/>
+      <c r="D884" s="8"/>
     </row>
     <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D885" s="7"/>
+      <c r="D885" s="8"/>
     </row>
     <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D886" s="7"/>
+      <c r="D886" s="8"/>
     </row>
     <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D887" s="7"/>
+      <c r="D887" s="8"/>
     </row>
     <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D888" s="7"/>
+      <c r="D888" s="8"/>
     </row>
     <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D889" s="7"/>
+      <c r="D889" s="8"/>
     </row>
     <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D890" s="7"/>
+      <c r="D890" s="8"/>
     </row>
     <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D891" s="7"/>
+      <c r="D891" s="8"/>
     </row>
     <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D892" s="7"/>
+      <c r="D892" s="8"/>
     </row>
     <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D893" s="7"/>
+      <c r="D893" s="8"/>
     </row>
     <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D894" s="7"/>
+      <c r="D894" s="8"/>
     </row>
     <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D895" s="7"/>
+      <c r="D895" s="8"/>
     </row>
     <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D896" s="7"/>
+      <c r="D896" s="8"/>
     </row>
     <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D897" s="7"/>
+      <c r="D897" s="8"/>
     </row>
     <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D898" s="7"/>
+      <c r="D898" s="8"/>
     </row>
     <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D899" s="7"/>
+      <c r="D899" s="8"/>
     </row>
     <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D900" s="7"/>
+      <c r="D900" s="8"/>
     </row>
     <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D901" s="7"/>
+      <c r="D901" s="8"/>
     </row>
     <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D902" s="7"/>
+      <c r="D902" s="8"/>
     </row>
     <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D903" s="7"/>
+      <c r="D903" s="8"/>
     </row>
     <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D904" s="7"/>
+      <c r="D904" s="8"/>
     </row>
     <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D905" s="7"/>
+      <c r="D905" s="8"/>
     </row>
     <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D906" s="7"/>
+      <c r="D906" s="8"/>
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D907" s="7"/>
+      <c r="D907" s="8"/>
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D908" s="7"/>
+      <c r="D908" s="8"/>
     </row>
     <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D909" s="7"/>
+      <c r="D909" s="8"/>
     </row>
     <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D910" s="7"/>
+      <c r="D910" s="8"/>
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D911" s="7"/>
+      <c r="D911" s="8"/>
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D912" s="7"/>
+      <c r="D912" s="8"/>
     </row>
     <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D913" s="7"/>
+      <c r="D913" s="8"/>
     </row>
     <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D914" s="7"/>
+      <c r="D914" s="8"/>
     </row>
     <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D915" s="7"/>
+      <c r="D915" s="8"/>
     </row>
     <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D916" s="7"/>
+      <c r="D916" s="8"/>
     </row>
     <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D917" s="7"/>
+      <c r="D917" s="8"/>
     </row>
     <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D918" s="7"/>
+      <c r="D918" s="8"/>
     </row>
     <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D919" s="7"/>
+      <c r="D919" s="8"/>
     </row>
     <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D920" s="7"/>
+      <c r="D920" s="8"/>
     </row>
     <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D921" s="7"/>
+      <c r="D921" s="8"/>
     </row>
     <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D922" s="7"/>
+      <c r="D922" s="8"/>
     </row>
     <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D923" s="7"/>
+      <c r="D923" s="8"/>
     </row>
     <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D924" s="7"/>
+      <c r="D924" s="8"/>
     </row>
     <row r="925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D925" s="7"/>
+      <c r="D925" s="8"/>
     </row>
     <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D926" s="7"/>
+      <c r="D926" s="8"/>
     </row>
     <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D927" s="7"/>
+      <c r="D927" s="8"/>
     </row>
     <row r="928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D928" s="7"/>
+      <c r="D928" s="8"/>
     </row>
     <row r="929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D929" s="7"/>
+      <c r="D929" s="8"/>
     </row>
     <row r="930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D930" s="7"/>
+      <c r="D930" s="8"/>
     </row>
     <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D931" s="7"/>
+      <c r="D931" s="8"/>
     </row>
     <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D932" s="7"/>
+      <c r="D932" s="8"/>
     </row>
     <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D933" s="7"/>
+      <c r="D933" s="8"/>
     </row>
     <row r="934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D934" s="7"/>
+      <c r="D934" s="8"/>
     </row>
     <row r="935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D935" s="7"/>
+      <c r="D935" s="8"/>
     </row>
     <row r="936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D936" s="7"/>
+      <c r="D936" s="8"/>
     </row>
     <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D937" s="7"/>
+      <c r="D937" s="8"/>
     </row>
     <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D938" s="7"/>
+      <c r="D938" s="8"/>
     </row>
     <row r="939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D939" s="7"/>
+      <c r="D939" s="8"/>
     </row>
     <row r="940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D940" s="7"/>
+      <c r="D940" s="8"/>
     </row>
     <row r="941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D941" s="7"/>
+      <c r="D941" s="8"/>
     </row>
     <row r="942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D942" s="7"/>
+      <c r="D942" s="8"/>
     </row>
     <row r="943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D943" s="7"/>
+      <c r="D943" s="8"/>
     </row>
     <row r="944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D944" s="7"/>
+      <c r="D944" s="8"/>
     </row>
     <row r="945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D945" s="7"/>
+      <c r="D945" s="8"/>
     </row>
     <row r="946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D946" s="7"/>
+      <c r="D946" s="8"/>
     </row>
     <row r="947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D947" s="7"/>
+      <c r="D947" s="8"/>
     </row>
     <row r="948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D948" s="7"/>
+      <c r="D948" s="8"/>
     </row>
     <row r="949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D949" s="7"/>
+      <c r="D949" s="8"/>
     </row>
     <row r="950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D950" s="7"/>
+      <c r="D950" s="8"/>
     </row>
     <row r="951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D951" s="7"/>
+      <c r="D951" s="8"/>
     </row>
     <row r="952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D952" s="7"/>
+      <c r="D952" s="8"/>
     </row>
     <row r="953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D953" s="7"/>
+      <c r="D953" s="8"/>
     </row>
     <row r="954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D954" s="7"/>
+      <c r="D954" s="8"/>
     </row>
     <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D955" s="7"/>
+      <c r="D955" s="8"/>
     </row>
     <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D956" s="7"/>
+      <c r="D956" s="8"/>
     </row>
     <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D957" s="7"/>
+      <c r="D957" s="8"/>
     </row>
     <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D958" s="7"/>
+      <c r="D958" s="8"/>
     </row>
     <row r="959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D959" s="7"/>
+      <c r="D959" s="8"/>
     </row>
     <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D960" s="7"/>
+      <c r="D960" s="8"/>
     </row>
     <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D961" s="7"/>
+      <c r="D961" s="8"/>
     </row>
     <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D962" s="7"/>
+      <c r="D962" s="8"/>
     </row>
     <row r="963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D963" s="7"/>
+      <c r="D963" s="8"/>
     </row>
     <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D964" s="7"/>
+      <c r="D964" s="8"/>
     </row>
     <row r="965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D965" s="7"/>
+      <c r="D965" s="8"/>
     </row>
     <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D966" s="7"/>
+      <c r="D966" s="8"/>
     </row>
     <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D967" s="7"/>
+      <c r="D967" s="8"/>
     </row>
     <row r="968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D968" s="7"/>
+      <c r="D968" s="8"/>
     </row>
     <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D969" s="7"/>
+      <c r="D969" s="8"/>
     </row>
     <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D970" s="7"/>
+      <c r="D970" s="8"/>
     </row>
     <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D971" s="7"/>
+      <c r="D971" s="8"/>
     </row>
     <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D972" s="7"/>
+      <c r="D972" s="8"/>
     </row>
     <row r="973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D973" s="7"/>
+      <c r="D973" s="8"/>
     </row>
     <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D974" s="7"/>
+      <c r="D974" s="8"/>
     </row>
     <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D975" s="7"/>
+      <c r="D975" s="8"/>
     </row>
     <row r="976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D976" s="7"/>
+      <c r="D976" s="8"/>
     </row>
     <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D977" s="7"/>
+      <c r="D977" s="8"/>
     </row>
     <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D978" s="7"/>
+      <c r="D978" s="8"/>
     </row>
     <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D979" s="7"/>
+      <c r="D979" s="8"/>
     </row>
     <row r="980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D980" s="7"/>
+      <c r="D980" s="8"/>
     </row>
     <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D981" s="7"/>
+      <c r="D981" s="8"/>
     </row>
     <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D982" s="7"/>
+      <c r="D982" s="8"/>
     </row>
     <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D983" s="7"/>
+      <c r="D983" s="8"/>
     </row>
     <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D984" s="7"/>
+      <c r="D984" s="8"/>
     </row>
     <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D985" s="7"/>
+      <c r="D985" s="8"/>
     </row>
     <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D986" s="7"/>
+      <c r="D986" s="8"/>
     </row>
     <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D987" s="7"/>
+      <c r="D987" s="8"/>
     </row>
     <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D988" s="7"/>
+      <c r="D988" s="8"/>
     </row>
     <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D989" s="7"/>
+      <c r="D989" s="8"/>
     </row>
     <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D990" s="7"/>
+      <c r="D990" s="8"/>
     </row>
     <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D991" s="7"/>
+      <c r="D991" s="8"/>
     </row>
     <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D992" s="7"/>
+      <c r="D992" s="8"/>
     </row>
     <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D993" s="7"/>
+      <c r="D993" s="8"/>
     </row>
     <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D994" s="7"/>
+      <c r="D994" s="8"/>
     </row>
     <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D995" s="7"/>
+      <c r="D995" s="8"/>
     </row>
     <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D996" s="7"/>
+      <c r="D996" s="8"/>
     </row>
     <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D997" s="7"/>
+      <c r="D997" s="8"/>
     </row>
     <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D998" s="7"/>
+      <c r="D998" s="8"/>
     </row>
     <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D999" s="7"/>
+      <c r="D999" s="8"/>
     </row>
     <row r="1000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1000" s="7"/>
+      <c r="D1000" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>